<commit_message>
Finalize self evaluation file
</commit_message>
<xml_diff>
--- a/docs/auto-avaliacao-g45.xlsx
+++ b/docs/auto-avaliacao-g45.xlsx
@@ -261,7 +261,7 @@
     <t xml:space="preserve">Observações:</t>
   </si>
   <si>
-    <t xml:space="preserve">Após discussão com o professor de Laboratório, foi determinado que (pelo menos no nosso Laboratório) a implementação de leitura do teclado em paralelo com sockets (via select) era opcional, pelo que não o implementámos.</t>
+    <t xml:space="preserve">Após discussão com o professor de Laboratório, foi determinado que (pelo menos no nosso Laboratório) a implementação de leitura do teclado em paralelo com sockets (via select) era opcional, pelo que não o implementámos. Seguindo essa mesma lógica, nunca haverão conexões TCP ativas (client-side) caso o player execute o comando exit, pelo que acabou por não ser uma preocupação da nossa parte no desenvolvimento do projeto.</t>
   </si>
   <si>
     <t xml:space="preserve">Execução correta dos scripts de testes do sevidor GS:</t>
@@ -515,12 +515,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -604,7 +608,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -628,8 +632,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FF2C2C2C"/>
+          <fgColor rgb="FFD3DAE3"/>
+          <bgColor rgb="FF404552"/>
         </patternFill>
       </fill>
     </dxf>
@@ -689,504 +693,504 @@
   </sheetPr>
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="4.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="47.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="47.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="2" width="4.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="47.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3"/>
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="n">
+      <c r="B5" s="8" t="n">
         <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="6"/>
+      <c r="B6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="11" t="n">
+      <c r="B7" s="12" t="n">
         <f aca="false">B8+F8</f>
         <v>20</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="2" t="n">
         <f aca="false">C8+G8</f>
         <v>20</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="12" t="n">
+      <c r="B8" s="13" t="n">
         <f aca="false">SUM(B9:B23)</f>
         <v>12</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="2" t="n">
         <f aca="false">SUM(C9:C23)</f>
         <v>12</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="12" t="n">
+      <c r="F8" s="13" t="n">
         <f aca="false">SUM(F9:F23)</f>
         <v>8</v>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="G8" s="2" t="n">
         <f aca="false">SUM(G9:G23)</f>
         <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="13" t="s">
+      <c r="B9" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="n">
+      <c r="F9" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" s="13" t="s">
+      <c r="B10" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1" t="n">
+      <c r="F10" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" s="13" t="s">
+      <c r="B11" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1" t="n">
+      <c r="F11" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" s="13" t="s">
+      <c r="B12" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="14" t="n">
+      <c r="F12" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="G12" s="1" t="n">
+      <c r="G12" s="2" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="7" t="n">
+      <c r="B14" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="C14" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1" t="n">
+      <c r="F14" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E15" s="13"/>
-      <c r="F15" s="12"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="E16" s="5" t="s">
+      <c r="B16" s="13"/>
+      <c r="E16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="7" t="n">
+      <c r="B18" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="C18" s="1" t="n">
+      <c r="C18" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1" t="n">
+      <c r="F18" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E19" s="13" t="s">
+      <c r="B19" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1" t="n">
+      <c r="F19" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E20" s="13" t="s">
+      <c r="B20" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="14" t="n">
+      <c r="F20" s="15" t="n">
         <v>0.5</v>
       </c>
-      <c r="G20" s="1" t="n">
+      <c r="G20" s="2" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="7" t="n">
+      <c r="B22" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="C22" s="1" t="n">
+      <c r="C22" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F22" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1" t="n">
+      <c r="F22" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="16" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="17"/>
-      <c r="B26" s="18"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="19"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="21" t="s">
+      <c r="A44" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="21" t="s">
+      <c r="A45" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="21" t="s">
+      <c r="A46" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="15" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1239,154 +1243,154 @@
       <selection pane="topLeft" activeCell="E44" activeCellId="0" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.93"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="23" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>0.25</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>0.25</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>0.25</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="J5" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>0.75</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="1" t="n">
         <v>0.75</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="J6" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="0" t="n">
+      <c r="F7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="1" t="n">
         <v>1.25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="1" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="1" t="n">
         <v>1.75</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="23" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="23" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="23" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="23" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>